<commit_message>
make test specific, add constraints on email, weight
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>weight_in_mgs</t>
+          <t>weight</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>weight_in_mgs</t>
+          <t>weight</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding some rules, id_prefixes, slot_usage
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -4,17 +4,19 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Animal" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NamedThing" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Person" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="PersonCollection" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Animal1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="NamedThing1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Person1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="PersonCollection1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AnimalCollection" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NamedThing" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Person" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PersonCollection" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Animal1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AnimalCollection1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="NamedThing1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Person1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="PersonCollection1" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,7 +468,33 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>weight</t>
+          <t>weight_in_mgs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
         </is>
       </c>
     </row>
@@ -481,6 +509,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>animals</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -516,7 +570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -533,6 +587,88 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>age_in_years</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>primary_email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>vital_status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>pets</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Person_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>entries</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -553,227 +689,145 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>breed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>weight_in_mgs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>animals</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>age_in_years</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>age_in_years</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>primary_email</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>vital_status</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>pets</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>pets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>species</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>breed</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>color</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>pets</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
+          <t>Person_id</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing test data inline with linter
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>

<commit_message>
updating according to linter
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -443,7 +443,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>

<commit_message>
fixing up with linter
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -443,7 +443,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>birth date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>

<commit_message>
bringing branch in line with downstream stuff
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_schema.xlsx
+++ b/project/excel/linkml_tutorial_schema.xlsx
@@ -4,15 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonCollection" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="NamedThing1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Person1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="PersonCollection1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Person" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Person1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,16 +428,6 @@
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -449,62 +435,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -521,125 +451,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>personCollection__entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>primary_email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>personCollection__entries</t>
         </is>
       </c>
     </row>

</xml_diff>